<commit_message>
add login and registration BR
</commit_message>
<xml_diff>
--- a/Testing/Reports/Car-BugReports.xlsx
+++ b/Testing/Reports/Car-BugReports.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Car-Bookings\Testing\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\QA project\Car-Bookings\Testing\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8790" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="add_car_bug_report" sheetId="1" r:id="rId1"/>
     <sheet name="update_car_bug_report" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Registration" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">update_car_bug_report!$A$1:$R$1</definedName>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -386,6 +388,184 @@
 car page will navigate you to the
  admin home page</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Test data</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Detected by</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>Attachements</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Bug_login_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The login form the password field default text is missing "Password"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Browser is opened successfully with updated version
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+ Login page URL: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://localhost:8080/New%20folder/login.php</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open The Login Page
+</t>
+  </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>1- The username field should have default text "Username"
+2- The password field should have default text "Password"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-The username field have default text "Username"
+2-There is not text inside password field
+</t>
+  </si>
+  <si>
+    <t>Eslam</t>
+  </si>
+  <si>
+    <t>24-5-2022</t>
+  </si>
+  <si>
+    <t>Bug_Reg_001</t>
+  </si>
+  <si>
+    <t>When user register there is  password formate validation required (8 characters at least and one uppercase  and one lowecase letters which is against what is written in SRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- browser is opened successfully
+- Registration page is accessed successfully
+</t>
+  </si>
+  <si>
+    <t>1- Email = "Eslam@fawzy.com"
+2- Phone = "01125669737"
+3- Password = "24233"
+4- Confirm Password = "24233"</t>
+  </si>
+  <si>
+    <t>1- Enter valid email format that doesn't exist in database 
+2- Enter valid phone number that consists of digits only
+3-enter password
+4-Enter the pre-entered password
+5-Click om register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aya </t>
+  </si>
+  <si>
+    <t>1- Confirm Registration by showing a message
+2- Send username through emaill</t>
+  </si>
+  <si>
+    <t>1- Error message when entering password that reqiures a specific formate (8 characters at least and one uppercase and onelower case letters)</t>
+  </si>
+  <si>
+    <t>Bug_Reg_002</t>
+  </si>
+  <si>
+    <t>When registering with email that already exists in database the error message that  appears is not understandable</t>
+  </si>
+  <si>
+    <t>1- Email = "aya@gmail.com"
+2-Phone = "01144942707"
+3- Password = "AYAtarek1"
+4-Password = "AYAtarek1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- enter valid email that exists in database
+2- enter valid phone number
+3-Enter valid password
+4-Enter the pre-entered password
+5-Click on register
+</t>
+  </si>
+  <si>
+    <t>1- Unsuccessful registration occur
+ 2- Error Message Will appear</t>
+  </si>
+  <si>
+    <t>1- The user register successfully</t>
+  </si>
+  <si>
+    <t>Bug_Reg_003</t>
+  </si>
+  <si>
+    <t>The default texts inside the email field is wrong "Write your mail"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-check text inside email field
+2-check text inside phone number field
+3- check text inside password field
+4-check text inside password cofirmation field
+</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>1-Text inside email field should be "Email"
+2-Text inside email field should be "Phone number"
+3- Text inside password field should be "Password"
+4- Text inside password confirmation field should be "Confirm password"</t>
+  </si>
+  <si>
+    <t>1-Text inside email field is "Write your mail"
+2-Text inside email field should be "Phone number"
+3- Text inside password field should be "Password"
+4- Text inside password confirmation field should be "Confirm password"</t>
+  </si>
+  <si>
+    <t>Bug_Reg_004</t>
+  </si>
+  <si>
+    <t>The login link does not redirect login page message "page not found" appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- click on login link in registration page
+</t>
+  </si>
 </sst>
 </file>
 
@@ -394,7 +574,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -464,8 +644,43 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,8 +710,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3CEFA"/>
+        <bgColor rgb="FFB3CEFA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -560,12 +781,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,9 +853,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,6 +877,51 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -857,7 +1144,7 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
@@ -883,10 +1170,10 @@
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
@@ -900,55 +1187,55 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="13"/>
@@ -962,47 +1249,47 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="182.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
       <c r="R3" s="14"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -1014,47 +1301,47 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="27" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
       <c r="R4" s="14"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -28247,4 +28534,1712 @@
   <autoFilter ref="A1:R1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="27" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+    </row>
+    <row r="2" spans="1:27" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="40"/>
+    </row>
+    <row r="4" spans="1:27" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+    </row>
+    <row r="6" spans="1:27" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
+    </row>
+    <row r="8" spans="1:27" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A7:N7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>